<commit_message>
INS final commit remaining unstaged changes
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC03_INS_CancerType-BreastCancer.xlsx
+++ b/InputFiles/INS/TC03_INS_CancerType-BreastCancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/gayathri26sep/Commons_Automation/InputFiles/INS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6E0268-076E-A54F-B644-5291923CB300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB5FCB-35C0-0945-BCA1-80297511A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="1900" windowWidth="25560" windowHeight="16260" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="4680" yWindow="1900" windowWidth="25560" windowHeight="16260" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,27 @@
     <t>TC03_INS_CancerType-BreastCancer_WebData.xlsx</t>
   </si>
   <si>
+    <t>SELECT DISTINCT 
+    prg.program_name AS "Program",
+  CASE
+    WHEN prg.program_link IS NOT NULL THEN prg.program_acronym
+        ELSE prg.program_link
+    END  AS "Website",
+    prg.focus_area AS "Special Topic",
+    prg.cancer_type AS "Cancer Type",
+ CASE 
+        WHEN prg.data_link IS NOT NULL THEN prg.program_acronym     
+        ELSE prg.data_link
+    END AS "Data Location Details" 
+FROM 
+    df_program prg
+WHERE 
+     prg.cancer_type LIKE '%Breast Cancer%'
+ORDER BY 
+    lower(prg.program_name) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>SELECT DISTINCT
     COUNT(DISTINCT prg.program_id) AS "Programs",
     COUNT(DISTINCT prj.project_id) AS "Projects",
@@ -85,13 +106,13 @@
 LEFT JOIN 
     df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-    prg.cancer_type LIKE '%Breast Cancer%'</t>
+    prg.cancer_type LIKE '%Breast Cancer%';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
     prj.project_id AS "Project ID", 
     prj.project_title AS "Project Title",
-    prj.org_name AS "Organization",
+    prj.project_org_name AS "Organization",
     prj.project_start_date AS "Project Start Date",
     prj.project_end_date AS "Project End Date"
 FROM 
@@ -116,7 +137,7 @@
     gnt.principal_investigators AS "Principal Investigators",
     gnt.program_officers AS "Program Officers",
     gnt.fiscal_year AS "Fiscal Year",
-    gnt.project_end_date AS "Project End Date"
+    gnt.grant_end_date AS "Project End Date"
 FROM 
     df_grant gnt
 LEFT JOIN 
@@ -126,7 +147,7 @@
 LEFT JOIN 
     df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-    prg.cancer_type LIKE '%Breast Cancer%'
+    prg.cancer_type  LIKE '%Breast Cancer%'
 ORDER BY 
     lower(gnt.grant_id) ASC
 LIMIT 100;</t>
@@ -134,7 +155,7 @@
   <si>
     <t>SELECT DISTINCT
     pub.pmid AS "PubMed ID", 
-    pub.title AS "Title",
+    pub.publication_title AS "Title",
     pub.authors AS "Authors",
     pub.publication_date AS "Publication Date",
     pub.cited_by AS "Cited By",
@@ -142,6 +163,7 @@
     WHEN pub.relative_citation_ratio = 0 THEN '0'
     WHEN pub.relative_citation_ratio = 7.0 THEN '7'
     WHEN pub.relative_citation_ratio = 2.0 THEN '2'
+  WHEN pub.relative_citation_ratio = 1.0 THEN '1'
     WHEN pub.relative_citation_ratio = ROUND(pub.relative_citation_ratio) THEN CAST(ROUND(pub.relative_citation_ratio) AS VARCHAR) 
     ELSE CAST(ROUND(pub.relative_citation_ratio, 2) AS VARCHAR)
 END AS "Relative Citation Ratio"
@@ -154,29 +176,9 @@
 LEFT JOIN 
     df_grant gnt ON prj.project_id = gnt."project.project_id"
 WHERE 
-     prg.cancer_type LIKE '%Breast Cancer%'
+     prg.cancer_type  LIKE '%Breast Cancer%'
 ORDER BY 
     lower(pub.pmid) ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT 
-    prg.program_name AS "Program",
-CASE
-    WHEN prg.program_link IS NOT NULL THEN prg.program_acronym
-        ELSE prg.program_link
-    END  AS "Website",
-    prg.focus_area AS "Focus Area",
-    prg.cancer_type AS "Cancer Type",
- CASE 
-        WHEN prg.data_link IS NOT NULL THEN prg.program_acronym     
-        ELSE prg.data_link
-    END AS "Data Location Details"
-FROM 
-    df_program prg WHERE 
-     prg.cancer_type LIKE '%Breast Cancer%'
-ORDER BY 
-    lower(prg.program_name) ASC
 LIMIT 100;</t>
   </si>
 </sst>
@@ -184,30 +186,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -253,20 +234,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -589,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,11 +595,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -640,16 +612,16 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="356" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -657,8 +629,8 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -670,7 +642,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>